<commit_message>
juiste url in cursus.service backlog
</commit_message>
<xml_diff>
--- a/Documenten/006 - User Story Map - ZV.xlsx
+++ b/Documenten/006 - User Story Map - ZV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\ZV_CursusAdministratie\Documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B9DB27A-8CBC-4A03-B817-CFC8C9FB0E5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DACE5226-4263-4C54-AFAD-22DA7E60F7B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-5790" windowWidth="29040" windowHeight="15840" tabRatio="411" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Backlog" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="123">
   <si>
     <t>Cursussen invoeren</t>
   </si>
@@ -540,12 +539,33 @@
     <t>naam, achternaam, adres, postcode, woonplaats en rekeinignummer of naam, achternaa, bedrijf (evt. Afdeling) en offertenummer
 of om te gebruiken in de communicatie met die cursist.</t>
   </si>
+  <si>
+    <t>0 - Project-structuur</t>
+  </si>
+  <si>
+    <t>Mappenstructuur maken</t>
+  </si>
+  <si>
+    <t>Mappenstructuur maken en Github inrichten</t>
+  </si>
+  <si>
+    <t>Databasestructuur aanmaken</t>
+  </si>
+  <si>
+    <t>Data versturen</t>
+  </si>
+  <si>
+    <t>Databasestructuur en cors opzetten</t>
+  </si>
+  <si>
+    <t>Backend, testbaar opzetten met repository pattern</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -598,8 +618,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -652,6 +686,16 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -759,13 +803,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -897,11 +943,17 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="6" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="4" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
     <cellStyle name="20% - Accent6" xfId="3" builtinId="50"/>
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
     <cellStyle name="40% - Accent4" xfId="2" builtinId="43"/>
+    <cellStyle name="Good" xfId="4" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="5" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -2161,10 +2213,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2209,153 +2261,141 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="48" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="48">
+        <v>1</v>
+      </c>
+      <c r="C2" s="48">
+        <v>0</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="48" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="B2">
+      <c r="B3" s="45">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C3" s="45">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="F3" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="45" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" s="45">
+        <v>1</v>
+      </c>
+      <c r="C4" s="45">
+        <v>1</v>
+      </c>
+      <c r="D4" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E4" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F4" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G4" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H4" s="45" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="5" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="B3">
+      <c r="B5" s="46">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C5" s="46">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D5" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E5" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F5" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H5" s="46" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="6" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="B4">
+      <c r="B6" s="46">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C6" s="46">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D6" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E6" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F6" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H6" s="46" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23" t="s">
+    <row r="7" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="B5" s="23">
+      <c r="B7" s="47">
         <v>2</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C7" s="47">
         <v>2</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D7" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E7" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F7" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G7" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" t="s">
-        <v>96</v>
-      </c>
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B7">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" t="s">
-        <v>79</v>
-      </c>
-      <c r="G7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="H7" s="47" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2364,33 +2404,33 @@
         <v>95</v>
       </c>
       <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
         <v>4</v>
       </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8" t="s">
-        <v>0</v>
-      </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="G8" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="H8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>95</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -2402,88 +2442,91 @@
         <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="H9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="23" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>95</v>
       </c>
-      <c r="B10" s="23">
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11">
         <v>5</v>
       </c>
-      <c r="C10" s="23">
+      <c r="C11">
         <v>2</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="D11" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>97</v>
+      </c>
+      <c r="G11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" s="23">
+        <v>5</v>
+      </c>
+      <c r="C12" s="23">
+        <v>2</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F12" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="23" t="s">
+      <c r="G12" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="23" t="s">
+      <c r="H12" s="23" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>98</v>
-      </c>
-      <c r="B11">
-        <v>6</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>98</v>
-      </c>
-      <c r="B12">
-        <v>7</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" t="s">
-        <v>56</v>
-      </c>
-      <c r="H12" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -2491,7 +2534,7 @@
         <v>98</v>
       </c>
       <c r="B13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -2503,47 +2546,44 @@
         <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="G13" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="H13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="23" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>98</v>
       </c>
-      <c r="B14" s="23">
-        <v>8</v>
-      </c>
-      <c r="C14" s="23">
+      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="C14">
         <v>1</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="G14" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="H14" s="23" t="s">
+      <c r="F14" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B15">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -2552,212 +2592,212 @@
         <v>4</v>
       </c>
       <c r="E15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>64</v>
+        <v>99</v>
+      </c>
+      <c r="G15" t="s">
+        <v>58</v>
       </c>
       <c r="H15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="16" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" s="23">
+        <v>8</v>
+      </c>
+      <c r="C16" s="23">
+        <v>1</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>100</v>
       </c>
-      <c r="B16">
-        <v>10</v>
-      </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-      <c r="D16" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" t="s">
-        <v>101</v>
-      </c>
-      <c r="G16" t="s">
-        <v>102</v>
-      </c>
-      <c r="H16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="B17" s="23">
-        <v>10</v>
-      </c>
-      <c r="C17" s="23">
-        <v>2</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="F17" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="G17" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="H17" s="23" t="s">
-        <v>22</v>
+      <c r="B17">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H17" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>101</v>
+      </c>
+      <c r="G18" t="s">
+        <v>102</v>
+      </c>
+      <c r="H18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" s="23">
+        <v>10</v>
+      </c>
+      <c r="C19" s="23">
+        <v>2</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="H19" s="23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>104</v>
       </c>
-      <c r="B18">
+      <c r="B20">
         <v>11</v>
       </c>
-      <c r="C18">
+      <c r="C20">
         <v>3</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D20" t="s">
         <v>7</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E20" t="s">
         <v>8</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F20" t="s">
         <v>8</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G20" t="s">
         <v>30</v>
       </c>
-      <c r="H18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>104</v>
-      </c>
-      <c r="B19">
-        <v>11</v>
-      </c>
-      <c r="C19">
-        <v>3</v>
-      </c>
-      <c r="D19" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19" t="s">
-        <v>31</v>
-      </c>
-      <c r="H19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="B20" s="23">
-        <v>11</v>
-      </c>
-      <c r="C20" s="23">
-        <v>3</v>
-      </c>
-      <c r="D20" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="H20" s="23" t="s">
+      <c r="H20" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B21">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="F21" t="s">
-        <v>70</v>
-      </c>
-      <c r="G21" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="H21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>106</v>
-      </c>
-      <c r="B22">
-        <v>12</v>
-      </c>
-      <c r="C22">
+    <row r="22" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="B22" s="23">
+        <v>11</v>
+      </c>
+      <c r="C22" s="23">
         <v>3</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="F22" t="s">
-        <v>41</v>
-      </c>
-      <c r="G22" t="s">
-        <v>42</v>
-      </c>
-      <c r="H22" t="s">
+      <c r="F22" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" s="23" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B23">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="E23" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="F23" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="G23" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="H23" t="s">
         <v>23</v>
@@ -2765,25 +2805,25 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B24">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F24" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="G24" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="H24" t="s">
         <v>23</v>
@@ -2791,25 +2831,25 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B25">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E25" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="F25" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G25" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="H25" t="s">
         <v>23</v>
@@ -2817,105 +2857,105 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B26">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E26" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F26" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G26" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="H26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="23" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>108</v>
       </c>
-      <c r="B27" s="23">
+      <c r="B27">
         <v>14</v>
       </c>
-      <c r="C27" s="23">
+      <c r="C27">
         <v>4</v>
       </c>
-      <c r="D27" s="23" t="s">
+      <c r="D27" t="s">
         <v>9</v>
       </c>
-      <c r="E27" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="F27" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="G27" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="H27" s="23" t="s">
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" t="s">
+        <v>43</v>
+      </c>
+      <c r="H27" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B28">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C28">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E28" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F28" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G28" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="H28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>109</v>
-      </c>
-      <c r="B29">
-        <v>15</v>
-      </c>
-      <c r="C29">
-        <v>3</v>
-      </c>
-      <c r="D29" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" t="s">
-        <v>21</v>
-      </c>
-      <c r="F29" t="s">
-        <v>50</v>
-      </c>
-      <c r="G29" t="s">
-        <v>51</v>
-      </c>
-      <c r="H29" t="s">
+    <row r="29" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" s="23">
+        <v>14</v>
+      </c>
+      <c r="C29" s="23">
+        <v>4</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="G29" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="H29" s="23" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2924,25 +2964,25 @@
         <v>109</v>
       </c>
       <c r="B30">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D30" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E30" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F30" t="s">
-        <v>105</v>
+        <v>8</v>
       </c>
       <c r="G30" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="H30" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -2950,51 +2990,51 @@
         <v>109</v>
       </c>
       <c r="B31">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E31" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F31" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="G31" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="H31" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B32">
         <v>16</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D32" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F32" t="s">
-        <v>8</v>
+        <v>105</v>
       </c>
       <c r="G32" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="H32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -3005,36 +3045,36 @@
         <v>16</v>
       </c>
       <c r="C33">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F33" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="G33" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="H33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B34">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E34" t="s">
         <v>8</v>
@@ -3043,7 +3083,7 @@
         <v>8</v>
       </c>
       <c r="G34" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="H34" t="s">
         <v>23</v>
@@ -3051,25 +3091,25 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B35">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C35">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E35" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F35" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H35" t="s">
         <v>23</v>
@@ -3077,16 +3117,16 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B36">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C36">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E36" t="s">
         <v>8</v>
@@ -3103,10 +3143,10 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B37">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C37">
         <v>3</v>
@@ -3118,12 +3158,64 @@
         <v>21</v>
       </c>
       <c r="F37" t="s">
+        <v>53</v>
+      </c>
+      <c r="G37" t="s">
+        <v>52</v>
+      </c>
+      <c r="H37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>111</v>
+      </c>
+      <c r="B38">
+        <v>18</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>19</v>
+      </c>
+      <c r="E38" t="s">
+        <v>8</v>
+      </c>
+      <c r="F38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" t="s">
+        <v>59</v>
+      </c>
+      <c r="H38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>111</v>
+      </c>
+      <c r="B39">
+        <v>19</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+      <c r="D39" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" t="s">
+        <v>21</v>
+      </c>
+      <c r="F39" t="s">
         <v>65</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G39" t="s">
         <v>66</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H39" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>